<commit_message>
Correct S10005, S10008, S10011
</commit_message>
<xml_diff>
--- a/tl/S10011.MES.BIN.xlsx
+++ b/tl/S10011.MES.BIN.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{231893F3-2157-4D7C-9604-2FFA0F3A27E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22036CE9-2B41-44D6-884B-AEE664B13D7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4530" yWindow="11820" windowWidth="49560" windowHeight="16875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -218,7 +218,7 @@
     <t>49</t>
   </si>
   <si>
-    <t>If I had to say it just for today, Eiji-san was is a really great person.</t>
+    <t>If I had to say it just for today, Eiji-san is a really great person.</t>
   </si>
   <si>
     <t>51</t>
@@ -659,7 +659,7 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>